<commit_message>
feat - filtro da matriz
- filtragem inicial pela matriz
- criação da lista dos clashs-semi-aprovados
- separação do txt pelos clashs semi-aprovados
</commit_message>
<xml_diff>
--- a/Matriz Clashs.xlsx
+++ b/Matriz Clashs.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://canhedobeppucombr.sharepoint.com/sites/Alemoa/Shared Documents/General/Matriz Clash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\geoconversor\Mês_2\Problema_dos_clashs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD85C57A-2282-423E-BB9E-F00CFA516786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{1716B75F-799A-4C5F-9E03-802481E07AF7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="2" r:id="rId1"/>
     <sheet name="Listagem" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="122">
   <si>
     <t>MATRIZ DE INTERFERÊNCIAS</t>
   </si>
@@ -397,12 +396,18 @@
   </si>
   <si>
     <t>Engastado</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -446,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -589,28 +594,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal style="thin">
-        <color indexed="64"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,28 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1023,410 +990,498 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305A38A7-3A88-4274-92DA-4C677BCE10F9}">
-  <dimension ref="A1:O15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="15" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.125" customWidth="1"/>
+    <col min="2" max="2" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="5.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:14">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="138">
+      <c r="B2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="24.75" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="24.75" customHeight="1" thickBot="1">
+      <c r="A12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="M13" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="129">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="87" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="21"/>
-    </row>
-    <row r="4" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="9"/>
-    </row>
-    <row r="6" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="9"/>
-    </row>
-    <row r="8" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="8"/>
-    </row>
-    <row r="9" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="9"/>
-    </row>
-    <row r="12" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="8"/>
-    </row>
-    <row r="13" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="9"/>
-    </row>
-    <row r="15" spans="1:15" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A15" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="12"/>
+      <c r="N13" s="17"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="M14" s="18"/>
+      <c r="N14" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="M13:N14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AB7059-AC1D-4A2D-B771-00A161F633CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.75" customWidth="1"/>
+    <col min="3" max="3" width="34.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2728,13 +2783,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9B636E-1D90-4291-AF4B-712D7133623B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9B636E-1D90-4291-AF4B-712D7133623B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46c1aeda-4339-4b8b-a459-7d103ad23afd"/>
+    <ds:schemaRef ds:uri="7f741f0e-0184-4da7-b34a-985725fbfc5c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24BE5561-D38A-4410-949A-27D5851D1DDF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24BE5561-D38A-4410-949A-27D5851D1DDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45B7DAC2-3615-4581-A9A5-5F14EE2CD8B7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45B7DAC2-3615-4581-A9A5-5F14EE2CD8B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="46c1aeda-4339-4b8b-a459-7d103ad23afd"/>
+    <ds:schemaRef ds:uri="7f741f0e-0184-4da7-b34a-985725fbfc5c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix - txt topografia e excel resolvido
</commit_message>
<xml_diff>
--- a/Matriz Clashs.xlsx
+++ b/Matriz Clashs.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="59">
   <si>
     <t>MATRIZ DE INTERFERÊNCIAS</t>
   </si>
@@ -125,9 +125,6 @@
     <t>T-HM-TERRENO</t>
   </si>
   <si>
-    <t>*Todos*</t>
-  </si>
-  <si>
     <t>Aprovado</t>
   </si>
   <si>
@@ -144,6 +141,78 @@
   </si>
   <si>
     <t>H-VALETA_CONCRETO</t>
+  </si>
+  <si>
+    <t>H_TRANSICAO_RET</t>
+  </si>
+  <si>
+    <t>H_TRANSICAO_TRAPEZ</t>
+  </si>
+  <si>
+    <t>H-BOCA_BUEIRO</t>
+  </si>
+  <si>
+    <t>H-BOCA_GALERIA</t>
+  </si>
+  <si>
+    <t>H-BUEIRO_CELULAR</t>
+  </si>
+  <si>
+    <t>H-CAIXA_COLETORA</t>
+  </si>
+  <si>
+    <t>H-CANALETA_CONCRETO</t>
+  </si>
+  <si>
+    <t>H-CRPP</t>
+  </si>
+  <si>
+    <t>H-DESCIDA_ENTRADA</t>
+  </si>
+  <si>
+    <t>H-DESCIDA_ESCADA</t>
+  </si>
+  <si>
+    <t>H-DESCIDA_RAPIDO</t>
+  </si>
+  <si>
+    <t>H-DISSIPADOR</t>
+  </si>
+  <si>
+    <t>H-GARGULA</t>
+  </si>
+  <si>
+    <t>H-HZ-CAIXA_EXISTENTE</t>
+  </si>
+  <si>
+    <t>H-MODULO A</t>
+  </si>
+  <si>
+    <t>H-MODULO B</t>
+  </si>
+  <si>
+    <t>H-MODULO C</t>
+  </si>
+  <si>
+    <t>H-MODULO D</t>
+  </si>
+  <si>
+    <t>H-SARJETA_GRAMA</t>
+  </si>
+  <si>
+    <t>H-TE_VALETA</t>
+  </si>
+  <si>
+    <t>H-TUBO DE QUEDA</t>
+  </si>
+  <si>
+    <t>H-TUBO_CONCRETO</t>
+  </si>
+  <si>
+    <t>GRAMA_PLACA</t>
+  </si>
+  <si>
+    <t>GRAMA_HIDROSSEMEADURA</t>
   </si>
 </sst>
 </file>
@@ -405,6 +474,24 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -416,24 +503,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,14 +1299,14 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="N13" s="17"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="M14" s="18"/>
-      <c r="N14" s="19"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1249,442 +1318,759 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="9.125" style="23"/>
+    <col min="1" max="1" width="14.625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.375" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="9.125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="A2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="D26" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="25" t="s">
+      <c r="B28" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="25" t="s">
+      <c r="E28" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="25" t="s">
+      <c r="C29" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
+      <c r="E29" s="20" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="20"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="20"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1692,6 +2078,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46c1aeda-4339-4b8b-a459-7d103ad23afd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7f741f0e-0184-4da7-b34a-985725fbfc5c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100420EFA20B37EED4A8F98A9C2EC890BB7" ma:contentTypeVersion="16" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="aea3d44a9351536121d93178e4f7fb0b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="46c1aeda-4339-4b8b-a459-7d103ad23afd" xmlns:ns3="7f741f0e-0184-4da7-b34a-985725fbfc5c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa4f8d974e4007d34fcdac288d761fe2" ns2:_="" ns3:_="">
     <xsd:import namespace="46c1aeda-4339-4b8b-a459-7d103ad23afd"/>
@@ -1932,27 +2338,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9B636E-1D90-4291-AF4B-712D7133623B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46c1aeda-4339-4b8b-a459-7d103ad23afd"/>
+    <ds:schemaRef ds:uri="7f741f0e-0184-4da7-b34a-985725fbfc5c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46c1aeda-4339-4b8b-a459-7d103ad23afd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7f741f0e-0184-4da7-b34a-985725fbfc5c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24BE5561-D38A-4410-949A-27D5851D1DDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45B7DAC2-3615-4581-A9A5-5F14EE2CD8B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1969,23 +2374,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24BE5561-D38A-4410-949A-27D5851D1DDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9B636E-1D90-4291-AF4B-712D7133623B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46c1aeda-4339-4b8b-a459-7d103ad23afd"/>
-    <ds:schemaRef ds:uri="7f741f0e-0184-4da7-b34a-985725fbfc5c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>